<commit_message>
New Cash Bill Added
</commit_message>
<xml_diff>
--- a/book.xlsx
+++ b/book.xlsx
@@ -8485,7 +8485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8580,25 +8580,19 @@
       <c r="G2" t="n">
         <v>11</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>222</t>
-        </is>
+      <c r="H2" t="n">
+        <v>222</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
           <t>cash</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>-211.0</t>
-        </is>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-211</v>
       </c>
     </row>
     <row r="3">
@@ -8631,23 +8625,68 @@
       <c r="G3" t="n">
         <v>200</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="H3" t="n">
+        <v>100</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>Cash</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="J3" t="n">
+        <v>0</v>
       </c>
       <c r="K3" t="n">
         <v>-111</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>21-09-22</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>qasim</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>923054129775</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>10 Kg Jutta</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>1020</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>-91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Cash Bill Added (#1)
</commit_message>
<xml_diff>
--- a/book.xlsx
+++ b/book.xlsx
@@ -8485,7 +8485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8580,25 +8580,19 @@
       <c r="G2" t="n">
         <v>11</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>222</t>
-        </is>
+      <c r="H2" t="n">
+        <v>222</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
           <t>cash</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>-211.0</t>
-        </is>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-211</v>
       </c>
     </row>
     <row r="3">
@@ -8631,23 +8625,68 @@
       <c r="G3" t="n">
         <v>200</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="H3" t="n">
+        <v>100</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>Cash</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="J3" t="n">
+        <v>0</v>
       </c>
       <c r="K3" t="n">
         <v>-111</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>21-09-22</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>qasim</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>923054129775</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>10 Kg Jutta</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>1020</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>-91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>